<commit_message>
Update: some preprocessing steps included to help generalize
</commit_message>
<xml_diff>
--- a/median_color_signatures.xlsx
+++ b/median_color_signatures.xlsx
@@ -481,42 +481,42 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>(117.0, 156.0, 175.0)</t>
+          <t>(188.0, 211.0, 220.0)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>(201.0, 236.0, 50.0)</t>
+          <t>(182.0, 216.0, 45.0)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>(240.0, 148.0, 23.0)</t>
+          <t>(245.0, 150.0, 5.0)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>(233.0, 172.0, 211.0)</t>
+          <t>(240.0, 192.0, 223.0)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>(184.0, 97.0, 76.0)</t>
+          <t>(186.0, 101.0, 78.0)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>(112.0, 113.0, 111.0)</t>
+          <t>(90.5, 97.5, 87.0)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>(219.0, 210.0, 214.0)</t>
+          <t>(230.0, 229.0, 225.0)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>(172.0, 158.0, 35.0)</t>
+          <t>(171.0, 158.0, 31.0)</t>
         </is>
       </c>
     </row>
@@ -526,38 +526,38 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(237.0, 254.0, 254.0)</t>
+          <t>(237.0, 253.0, 254.0)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>(129.0, 195.0, 122.0)</t>
+          <t>(128.0, 199.5, 122.0)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>(252.0, 160.0, 251.0)</t>
+          <t>(255.0, 157.0, 255.0)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>(245.0, 61.0, 62.0)</t>
+          <t>(254.0, 80.0, 60.0)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>(116.0, 115.0, 114.0)</t>
+          <t>(113.0, 110.0, 108.0)</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>(219.0, 219.0, 217.0)</t>
+          <t>(228.0, 228.0, 227.0)</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>(253.0, 243.0, 39.0)</t>
+          <t>(254.0, 255.0, 53.0)</t>
         </is>
       </c>
     </row>
@@ -567,7 +567,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(223.0, 232.0, 240.0)</t>
+          <t>(227.0, 235.0, 242.0)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -576,17 +576,17 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>(128.0, 120.0, 107.0)</t>
+          <t>(136.0, 130.0, 123.0)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>(230.0, 228.0, 223.0)</t>
+          <t>(235.0, 234.0, 230.0)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>(114.0, 84.0, 33.0)</t>
+          <t>(126.0, 86.0, 32.0)</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>(209.0, 226.0, 238.0)</t>
+          <t>(226.0, 235.0, 241.0)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -605,12 +605,12 @@
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>(140.0, 136.0, 129.0)</t>
+          <t>(137.0, 132.0, 124.0)</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>(236.0, 235.0, 237.0)</t>
+          <t>(233.0, 232.0, 234.0)</t>
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
@@ -621,7 +621,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>(68.0, 171.0, 223.0)</t>
+          <t>(169.0, 217.0, 243.0)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -630,12 +630,12 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>(133.0, 128.0, 113.0)</t>
+          <t>(138.0, 132.0, 118.0)</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>(239.0, 237.0, 239.0)</t>
+          <t>(237.0, 236.0, 238.0)</t>
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
@@ -646,7 +646,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>(150.0, 198.0, 240.0)</t>
+          <t>(167.0, 208.0, 244.0)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -655,12 +655,12 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>(110.0, 102.0, 91.0)</t>
+          <t>(136.0, 127.5, 115.0)</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>(227.0, 227.0, 234.0)</t>
+          <t>(225.0, 225.0, 233.0)</t>
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
@@ -671,7 +671,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>(180.0, 210.0, 232.5)</t>
+          <t>(224.0, 235.0, 240.0)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -688,7 +688,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>(172.0, 208.0, 246.0)</t>
+          <t>(184.0, 217.0, 250.0)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -705,7 +705,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>(45.5, 152.0, 226.0)</t>
+          <t>(35.0, 158.0, 235.0)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -722,7 +722,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>(39.0, 141.0, 207.0)</t>
+          <t>(41.0, 144.0, 211.0)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -739,7 +739,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>(241.0, 254.0, 255.0)</t>
+          <t>(242.0, 254.0, 254.0)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -756,7 +756,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>(227.0, 246.0, 253.0)</t>
+          <t>(226.0, 245.0, 252.0)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -773,7 +773,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>(233.0, 248.0, 253.0)</t>
+          <t>(241.0, 253.0, 253.0)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -790,7 +790,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>(240.0, 254.0, 254.0)</t>
+          <t>(239.0, 254.0, 253.0)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -807,7 +807,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>(205.0, 228.0, 240.0)</t>
+          <t>(202.0, 226.0, 238.0)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>(200.0, 230.0, 234.0)</t>
+          <t>(197.0, 227.0, 232.0)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -841,7 +841,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>(231.0, 240.0, 248.0)</t>
+          <t>(229.0, 239.0, 248.0)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -858,7 +858,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>(218.0, 251.0, 240.0)</t>
+          <t>(247.0, 255.0, 254.0)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>

</xml_diff>